<commit_message>
Fixing a bug with user login, updating styles and adding income and expense prediction
</commit_message>
<xml_diff>
--- a/Users/Datas/EgorAndrik.xlsx
+++ b/Users/Datas/EgorAndrik.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,21 @@
           <t>income_or_expenses</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>CNY</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -457,12 +472,21 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>expenses</t>
         </is>
+      </c>
+      <c r="D2" t="n">
+        <v>96.33</v>
+      </c>
+      <c r="E2" t="n">
+        <v>104.94</v>
+      </c>
+      <c r="F2" t="n">
+        <v>13.19</v>
       </c>
     </row>
     <row r="3">
@@ -472,147 +496,237 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>350</v>
+        <v>500</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>expenses</t>
         </is>
+      </c>
+      <c r="D3" t="n">
+        <v>96.62</v>
+      </c>
+      <c r="E3" t="n">
+        <v>104.42</v>
+      </c>
+      <c r="F3" t="n">
+        <v>13.29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-09-09</t>
+          <t>2023-09-25</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>expenses</t>
         </is>
+      </c>
+      <c r="D4" t="n">
+        <v>96.04000000000001</v>
+      </c>
+      <c r="E4" t="n">
+        <v>102.25</v>
+      </c>
+      <c r="F4" t="n">
+        <v>13.14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>2023-10-10</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>195</v>
+        <v>2500</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>expenses</t>
         </is>
+      </c>
+      <c r="D5" t="n">
+        <v>101.36</v>
+      </c>
+      <c r="E5" t="n">
+        <v>107.03</v>
+      </c>
+      <c r="F5" t="n">
+        <v>13.89</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-09-23</t>
+          <t>2023-10-15</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>220</v>
+        <v>565</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>expenses</t>
         </is>
+      </c>
+      <c r="D6" t="n">
+        <v>97.31</v>
+      </c>
+      <c r="E6" t="n">
+        <v>102.55</v>
+      </c>
+      <c r="F6" t="n">
+        <v>13.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-09-30</t>
+          <t>2023-10-30</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>expenses</t>
         </is>
+      </c>
+      <c r="D7" t="n">
+        <v>93.22</v>
+      </c>
+      <c r="E7" t="n">
+        <v>98.34999999999999</v>
+      </c>
+      <c r="F7" t="n">
+        <v>12.71</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-09-01</t>
+          <t>2023-11-03</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>income</t>
-        </is>
+          <t>expenses</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>93.17</v>
+      </c>
+      <c r="E8" t="n">
+        <v>99</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-09-03</t>
+          <t>2023-09-01</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>550</v>
+        <v>1500</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>income</t>
         </is>
+      </c>
+      <c r="D9" t="n">
+        <v>96.33</v>
+      </c>
+      <c r="E9" t="n">
+        <v>104.94</v>
+      </c>
+      <c r="F9" t="n">
+        <v>13.19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-09-08</t>
+          <t>2023-09-02</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>income</t>
         </is>
+      </c>
+      <c r="D10" t="n">
+        <v>96.34</v>
+      </c>
+      <c r="E10" t="n">
+        <v>104.61</v>
+      </c>
+      <c r="F10" t="n">
+        <v>13.25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-09-09</t>
+          <t>2023-09-25</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50</v>
+        <v>2500</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>income</t>
         </is>
+      </c>
+      <c r="D11" t="n">
+        <v>96.04000000000001</v>
+      </c>
+      <c r="E11" t="n">
+        <v>102.25</v>
+      </c>
+      <c r="F11" t="n">
+        <v>13.14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-09-26</t>
+          <t>2023-09-30</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>333</v>
+        <v>5500</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>income</t>
         </is>
+      </c>
+      <c r="D12" t="n">
+        <v>97.41</v>
+      </c>
+      <c r="E12" t="n">
+        <v>103.16</v>
+      </c>
+      <c r="F12" t="n">
+        <v>13.36</v>
       </c>
     </row>
     <row r="13">
@@ -622,12 +736,45 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>income</t>
         </is>
+      </c>
+      <c r="D13" t="n">
+        <v>97.41</v>
+      </c>
+      <c r="E13" t="n">
+        <v>103.16</v>
+      </c>
+      <c r="F13" t="n">
+        <v>13.36</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-10-15</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>250</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>97.31</v>
+      </c>
+      <c r="E14" t="n">
+        <v>102.55</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug for styles
</commit_message>
<xml_diff>
--- a/Users/Datas/EgorAndrik.xlsx
+++ b/Users/Datas/EgorAndrik.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,59 +636,59 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-09-01</t>
+          <t>2023-11-07</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1500</v>
+        <v>30</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>expenses</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>96.33</v>
+        <v>93.04000000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>104.94</v>
+        <v>99.01000000000001</v>
       </c>
       <c r="F9" t="n">
-        <v>13.19</v>
+        <v>12.69</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-09-02</t>
+          <t>2023-11-10</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>expenses</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>96.34</v>
+        <v>91.93000000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>104.61</v>
+        <v>98.41</v>
       </c>
       <c r="F10" t="n">
-        <v>13.25</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-09-25</t>
+          <t>2023-09-01</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -696,23 +696,23 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>96.04000000000001</v>
+        <v>96.33</v>
       </c>
       <c r="E11" t="n">
-        <v>102.25</v>
+        <v>104.94</v>
       </c>
       <c r="F11" t="n">
-        <v>13.14</v>
+        <v>13.19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-09-30</t>
+          <t>2023-09-02</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5500</v>
+        <v>500</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -720,23 +720,23 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>97.41</v>
+        <v>96.34</v>
       </c>
       <c r="E12" t="n">
-        <v>103.16</v>
+        <v>104.61</v>
       </c>
       <c r="F12" t="n">
-        <v>13.36</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
+          <t>2023-09-25</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -744,37 +744,133 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>97.41</v>
+        <v>96.04000000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>103.16</v>
+        <v>102.25</v>
       </c>
       <c r="F13" t="n">
-        <v>13.36</v>
+        <v>13.14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>2023-09-30</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5500</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>97.41</v>
+      </c>
+      <c r="E14" t="n">
+        <v>103.16</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13.36</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>97.41</v>
+      </c>
+      <c r="E15" t="n">
+        <v>103.16</v>
+      </c>
+      <c r="F15" t="n">
+        <v>13.36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>2023-10-15</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B16" t="n">
         <v>250</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>income</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D16" t="n">
         <v>97.31</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E16" t="n">
         <v>102.55</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F16" t="n">
         <v>13.3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>25</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>92.02</v>
+      </c>
+      <c r="E17" t="n">
+        <v>97.93000000000001</v>
+      </c>
+      <c r="F17" t="n">
+        <v>12.53</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-11-11</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>92.05</v>
+      </c>
+      <c r="E18" t="n">
+        <v>98.31999999999999</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>